<commit_message>
Half string mediums done
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Chirag\STUDY\DSA\DSA 45 DAYS CHALLENGE\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2EC2EA9-E665-4C80-8985-3AB91CF3D59B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B27DA593-25AD-41C4-9DE5-E58DFF022027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{963251A3-5840-4013-B535-D0729DB36711}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="334">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="334">
   <si>
     <t>#DSASheetbyArsh (45-60 Days) : Sheet1</t>
   </si>
@@ -1607,8 +1607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{345952D3-C619-4DB6-A548-54F57AD92A84}">
   <dimension ref="A1:J335"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B28" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" topLeftCell="B34" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2432,7 +2432,9 @@
       <c r="D41" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="E41" s="5"/>
+      <c r="E41" s="22" t="s">
+        <v>332</v>
+      </c>
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
       <c r="H41" s="5"/>
@@ -2452,7 +2454,9 @@
       <c r="D42" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="E42" s="5"/>
+      <c r="E42" s="22" t="s">
+        <v>332</v>
+      </c>
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>
       <c r="H42" s="5"/>
@@ -2470,7 +2474,9 @@
       <c r="D43" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="E43" s="5"/>
+      <c r="E43" s="22" t="s">
+        <v>332</v>
+      </c>
       <c r="F43" s="13" t="s">
         <v>23</v>
       </c>
@@ -2492,7 +2498,9 @@
       <c r="D44" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="E44" s="5"/>
+      <c r="E44" s="22" t="s">
+        <v>332</v>
+      </c>
       <c r="F44" s="13" t="s">
         <v>23</v>
       </c>
@@ -2512,7 +2520,9 @@
       <c r="D45" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="E45" s="5"/>
+      <c r="E45" s="22" t="s">
+        <v>332</v>
+      </c>
       <c r="F45" s="12"/>
       <c r="G45" s="5"/>
       <c r="H45" s="5"/>
@@ -2532,7 +2542,9 @@
       <c r="D46" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="E46" s="5"/>
+      <c r="E46" s="22" t="s">
+        <v>332</v>
+      </c>
       <c r="F46" s="13" t="s">
         <v>23</v>
       </c>
@@ -2572,7 +2584,9 @@
       <c r="D48" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="E48" s="5"/>
+      <c r="E48" s="22" t="s">
+        <v>332</v>
+      </c>
       <c r="F48" s="13" t="s">
         <v>23</v>
       </c>

</xml_diff>